<commit_message>
Changes made to implement functionality to export sales entries to a PDF format.
</commit_message>
<xml_diff>
--- a/JournalEntries.xlsx
+++ b/JournalEntries.xlsx
@@ -6,17 +6,17 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="4_2022" r:id="rId3" sheetId="1"/>
-    <sheet name="5_2022" r:id="rId4" sheetId="2"/>
-    <sheet name="6_2022" r:id="rId5" sheetId="3"/>
-    <sheet name="7_2022" r:id="rId6" sheetId="4"/>
-    <sheet name="9_2022" r:id="rId7" sheetId="5"/>
-    <sheet name="10_2022" r:id="rId8" sheetId="6"/>
-    <sheet name="11_2022" r:id="rId9" sheetId="7"/>
-    <sheet name="12_2022" r:id="rId10" sheetId="8"/>
-    <sheet name="1_2023" r:id="rId11" sheetId="9"/>
-    <sheet name="2_2023" r:id="rId12" sheetId="10"/>
-    <sheet name="3_2023" r:id="rId13" sheetId="11"/>
+    <sheet name="APRIL_2022" r:id="rId3" sheetId="1"/>
+    <sheet name="MAY_2022" r:id="rId4" sheetId="2"/>
+    <sheet name="JUNE_2022" r:id="rId5" sheetId="3"/>
+    <sheet name="JULY_2022" r:id="rId6" sheetId="4"/>
+    <sheet name="SEPTEMBER_2022" r:id="rId7" sheetId="5"/>
+    <sheet name="OCTOBER_2022" r:id="rId8" sheetId="6"/>
+    <sheet name="NOVEMBER_2022" r:id="rId9" sheetId="7"/>
+    <sheet name="DECEMBER_2022" r:id="rId10" sheetId="8"/>
+    <sheet name="JANUARY_2023" r:id="rId11" sheetId="9"/>
+    <sheet name="FEBRUARY_2023" r:id="rId12" sheetId="10"/>
+    <sheet name="MARCH_2023" r:id="rId13" sheetId="11"/>
   </sheets>
 </workbook>
 </file>

</xml_diff>